<commit_message>
Organized Files that have been tracked and completed some vein based fitting.  Still need to finish veins fitting
</commit_message>
<xml_diff>
--- a/FlowTracker.xlsx
+++ b/FlowTracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cbnor\Documents\Full Body Flow Model Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E06C9B3A-287E-414B-AA92-50904D078601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{100621D6-8B41-49AC-8A82-C1CE039474E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{47D125F6-3825-4931-A32B-8D8704670F39}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{47D125F6-3825-4931-A32B-8D8704670F39}"/>
   </bookViews>
   <sheets>
     <sheet name="arteries" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1746" uniqueCount="723">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1826" uniqueCount="764">
   <si>
     <t>Filename</t>
   </si>
@@ -2206,6 +2206,129 @@
   </si>
   <si>
     <t>arteries_rleg19, arteries_rleg11, arteries_rleg8</t>
+  </si>
+  <si>
+    <t>left_subclavian_vein</t>
+  </si>
+  <si>
+    <t>IN Point</t>
+  </si>
+  <si>
+    <t>veins0</t>
+  </si>
+  <si>
+    <t>veins1</t>
+  </si>
+  <si>
+    <t>veins2</t>
+  </si>
+  <si>
+    <t>veins3</t>
+  </si>
+  <si>
+    <t>veins4</t>
+  </si>
+  <si>
+    <t>veins5</t>
+  </si>
+  <si>
+    <t>veins6</t>
+  </si>
+  <si>
+    <t>veins7</t>
+  </si>
+  <si>
+    <t>veins8</t>
+  </si>
+  <si>
+    <t>veins9</t>
+  </si>
+  <si>
+    <t>veins10</t>
+  </si>
+  <si>
+    <t>veins11</t>
+  </si>
+  <si>
+    <t>veins12</t>
+  </si>
+  <si>
+    <t>veins13</t>
+  </si>
+  <si>
+    <t>veins14</t>
+  </si>
+  <si>
+    <t>veins15</t>
+  </si>
+  <si>
+    <t>veins16</t>
+  </si>
+  <si>
+    <t>veins17</t>
+  </si>
+  <si>
+    <t>veins18</t>
+  </si>
+  <si>
+    <t>veins19</t>
+  </si>
+  <si>
+    <t>veins20</t>
+  </si>
+  <si>
+    <t>veins21</t>
+  </si>
+  <si>
+    <t>veins22</t>
+  </si>
+  <si>
+    <t>veins23</t>
+  </si>
+  <si>
+    <t>veins24</t>
+  </si>
+  <si>
+    <t>veins25</t>
+  </si>
+  <si>
+    <t>veins26</t>
+  </si>
+  <si>
+    <t>veins27</t>
+  </si>
+  <si>
+    <t>veins28</t>
+  </si>
+  <si>
+    <t>veins29</t>
+  </si>
+  <si>
+    <t>veins30</t>
+  </si>
+  <si>
+    <t>veins31</t>
+  </si>
+  <si>
+    <t>veins32</t>
+  </si>
+  <si>
+    <t>veins33</t>
+  </si>
+  <si>
+    <t>left_brachiocephalic_vein</t>
+  </si>
+  <si>
+    <t>right_barchiocephalic_vein</t>
+  </si>
+  <si>
+    <t>left_jugular_vein</t>
+  </si>
+  <si>
+    <t>left_brachiocephalic_vein, veins8,</t>
+  </si>
+  <si>
+    <t>veins11, veins3</t>
   </si>
 </sst>
 </file>
@@ -2253,10 +2376,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2573,9 +2695,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CF27AB3-E048-4EA5-B18B-CA67C65A1148}">
   <dimension ref="A1:G586"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A662" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2621,7 +2743,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="1"/>
-      <c r="E2" s="2" t="s">
+      <c r="E2" t="s">
         <v>717</v>
       </c>
       <c r="G2" t="s">
@@ -2773,7 +2895,6 @@
       <c r="C13" t="s">
         <v>81</v>
       </c>
-      <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
@@ -3298,7 +3419,7 @@
       <c r="D55" t="s">
         <v>103</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="E55" t="s">
         <v>102</v>
       </c>
     </row>
@@ -9022,12 +9143,342 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FF2BB04-6248-456D-B696-D17DD71C1F29}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.46484375" customWidth="1"/>
+    <col min="2" max="2" width="28.19921875" customWidth="1"/>
+    <col min="3" max="3" width="37" customWidth="1"/>
+    <col min="4" max="4" width="18.53125" customWidth="1"/>
+    <col min="5" max="5" width="18.19921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>724</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>642</v>
+      </c>
+      <c r="E4" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>725</v>
+      </c>
+      <c r="B6" t="s">
+        <v>761</v>
+      </c>
+      <c r="C6" t="s">
+        <v>729</v>
+      </c>
+      <c r="D6" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>726</v>
+      </c>
+      <c r="B7" t="s">
+        <v>759</v>
+      </c>
+      <c r="C7" t="s">
+        <v>723</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>728</v>
+      </c>
+      <c r="B9" t="s">
+        <v>728</v>
+      </c>
+      <c r="D9" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>729</v>
+      </c>
+      <c r="B10" t="s">
+        <v>729</v>
+      </c>
+      <c r="D10" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>730</v>
+      </c>
+      <c r="B11" t="s">
+        <v>723</v>
+      </c>
+      <c r="C11" t="s">
+        <v>732</v>
+      </c>
+      <c r="D11" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>732</v>
+      </c>
+      <c r="B13" t="s">
+        <v>732</v>
+      </c>
+      <c r="D13" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>733</v>
+      </c>
+      <c r="B14" t="s">
+        <v>733</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>734</v>
+      </c>
+      <c r="B15" t="s">
+        <v>760</v>
+      </c>
+      <c r="C15" t="s">
+        <v>763</v>
+      </c>
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>736</v>
+      </c>
+      <c r="B17" t="s">
+        <v>736</v>
+      </c>
+      <c r="D17" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>758</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Gettin' her done on Sat
</commit_message>
<xml_diff>
--- a/FlowTracker.xlsx
+++ b/FlowTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cbnor\Documents\Full Body Flow Model Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD7C7C4C-8133-46A1-995E-054F8527980A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FBC7331-9B98-4E6B-AD05-9315A3695AEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{47D125F6-3825-4931-A32B-8D8704670F39}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1933" uniqueCount="784">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2153" uniqueCount="822">
   <si>
     <t>Filename</t>
   </si>
@@ -2373,9 +2373,6 @@
     <t>right_pulmonary_art24, right_pulmonary_art26, right_pulmonary_art193</t>
   </si>
   <si>
-    <t>right_pulmonary_art191, right_pulmonary_art190, right_pulmonary_art23, right_pulmonary_art55</t>
-  </si>
-  <si>
     <t>right_pulmonary_art168, right_pulmonary_art169</t>
   </si>
   <si>
@@ -2389,6 +2386,123 @@
   </si>
   <si>
     <t>right_pulmonary_art71, right_pulmonary_art175</t>
+  </si>
+  <si>
+    <t>right_pulmonary_art21, right_pulmonary_art27, right_pulmonary_art41, right_pulmonary_art62, right_pulmonary_art116, right_pulmonary_art62, right_pulmonary_art119, right_pulmonary_art121</t>
+  </si>
+  <si>
+    <t xml:space="preserve">right_pulmonary_art117, right_pulmonary_art118 </t>
+  </si>
+  <si>
+    <t>right_pulmonary_art125, right_pulmonary_art104, right_pulmonary_art122, right_pulmonary_art123</t>
+  </si>
+  <si>
+    <t>right_pulmonary_art124, right_pulmonary_art52</t>
+  </si>
+  <si>
+    <t>right_pulmonary_art134, right_pulmonary_art40</t>
+  </si>
+  <si>
+    <t>right_pulmonary_art92, right_pulmonary_art102, right_pulmonary_art15, right_pulmonary_art16</t>
+  </si>
+  <si>
+    <t>right_pulmonary_art3, right_pulmonary_art101, right_pulmonary_art5, right_pulmonary_art6, right_pulmonary_art4, right_pulmonary_art160</t>
+  </si>
+  <si>
+    <t>right_pulmonary_art89, right_pulmonary_art109</t>
+  </si>
+  <si>
+    <t>right_pulmonary_art103, right_pulmonary_art157, right_pulmonary_art158, right_pulmonary_art159, right_pulmonary_art211</t>
+  </si>
+  <si>
+    <t>right_pulmonary_art209, right_pulmonary_art96</t>
+  </si>
+  <si>
+    <t>right_pulmonary_art42, right_pulmonary_art58, right_pulmonary_art87, right_pulmonary_art140, right_pulmonary_art170</t>
+  </si>
+  <si>
+    <t>right_pulmonary_art156, right_pulmonary_art86</t>
+  </si>
+  <si>
+    <t>right_pulmonary_art163, right_pulmonary_art105, right_pulmonary_art108</t>
+  </si>
+  <si>
+    <t>right_pulmonary_art105, right_pulmonary_art108</t>
+  </si>
+  <si>
+    <t>right_pulmonary_art155, right_pulmonary_art88</t>
+  </si>
+  <si>
+    <t>right_pulmonary_art153, right_pulmonary_art154</t>
+  </si>
+  <si>
+    <t>right_pulmonary_art49, right_pulmonary_art135, right_pulmonary_art136, right_pulmonary_art72, right_pulmonary_art137, right_pulmonary_art138, right_pulmonary_art139</t>
+  </si>
+  <si>
+    <t>right_pulmonary_art73, right_pulmonary_art74</t>
+  </si>
+  <si>
+    <t>right_pulmonary_art32, right_pulmonary_art33</t>
+  </si>
+  <si>
+    <t>right_pulmonary_art131, right_pulmonary_art68</t>
+  </si>
+  <si>
+    <t>right_pulmonary_art130, right_pulmonary_art48</t>
+  </si>
+  <si>
+    <t>right_pulmonary_art63, right_pulmonary_art66</t>
+  </si>
+  <si>
+    <t>right_pulmonary_art7, right_pulmonary_art14, right_pulmonary_art196, right_pulmonary_art18</t>
+  </si>
+  <si>
+    <t>right_pulmonary_art98, right_pulmonary_art97, right_pulmonary_art198, right_pulmonary_art199, right_pulmonary_art200, right_pulmonary_art205</t>
+  </si>
+  <si>
+    <t>right_pulmonary_art197, right_pulmonary_art95, right_pulmonary_art107</t>
+  </si>
+  <si>
+    <t>right_pulmonary_art95, right_pulmonary_art107</t>
+  </si>
+  <si>
+    <t>right_pulmonary_art99, right_pulmonary_art204</t>
+  </si>
+  <si>
+    <t>right_pulmonary_art203, right_pulmonary_art94</t>
+  </si>
+  <si>
+    <t>right_pulmonary_art202, right_pulmonary_art201</t>
+  </si>
+  <si>
+    <t>right_pulmonary_art2, right_pulmonary_art161, right_pulmonary_art11, right_pulmonary_art8, right_pulmonary_art12, right_pulmonary_art214</t>
+  </si>
+  <si>
+    <t>right_pulmonary_art212, right_pulmonary_art114</t>
+  </si>
+  <si>
+    <t>right_pulmonary_art81, right_pulmonary_art100, right_pulmonary_art84, right_pulmonary_art113, right_pulmonary_art10</t>
+  </si>
+  <si>
+    <t>right_pulmonary_art9, right_pulmonary_art83</t>
+  </si>
+  <si>
+    <t>right_pulmonary_art17, right_pulmonary_art93, right_pulmonary_art213</t>
+  </si>
+  <si>
+    <t>right_pulmonary_art208, right_pulmonary_art206</t>
+  </si>
+  <si>
+    <t>right_pulmonary_art90, right_pulmonary_art184</t>
+  </si>
+  <si>
+    <t>right_pulmonary_art128, right_pulmonary_art127, right_pulmonary_art126, right_pulmonary_art50, right_pulmonary_art30</t>
+  </si>
+  <si>
+    <t>right_pulmonary_art29, right_pulmonary_art47</t>
+  </si>
+  <si>
+    <t>right_pulmonary_art191, right_pulmonary_art190, right_pulmonary_art23, right_pulmonary_art55, right_pulmonary_art54</t>
   </si>
 </sst>
 </file>
@@ -2771,8 +2885,8 @@
   <dimension ref="A1:G586"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A367" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D379" sqref="D379"/>
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H67" sqref="H67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3673,6 +3787,9 @@
       <c r="C68" t="s">
         <v>114</v>
       </c>
+      <c r="G68" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
@@ -3684,6 +3801,9 @@
       <c r="C69" t="s">
         <v>118</v>
       </c>
+      <c r="G69" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
@@ -3698,6 +3818,9 @@
       <c r="D70" t="s">
         <v>119</v>
       </c>
+      <c r="G70" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
@@ -3709,6 +3832,9 @@
       <c r="C71" t="s">
         <v>115</v>
       </c>
+      <c r="G71" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
@@ -3720,6 +3846,9 @@
       <c r="C72" t="s">
         <v>114</v>
       </c>
+      <c r="G72" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
@@ -3734,6 +3863,9 @@
       <c r="D73" t="s">
         <v>115</v>
       </c>
+      <c r="G73" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
@@ -6716,7 +6848,7 @@
         <v>449</v>
       </c>
       <c r="D308" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="309" spans="1:7" x14ac:dyDescent="0.45">
@@ -6743,6 +6875,9 @@
       <c r="B310" t="s">
         <v>423</v>
       </c>
+      <c r="C310" t="s">
+        <v>435</v>
+      </c>
     </row>
     <row r="311" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A311" t="s">
@@ -6751,6 +6886,12 @@
       <c r="B311" t="s">
         <v>424</v>
       </c>
+      <c r="C311" t="s">
+        <v>637</v>
+      </c>
+      <c r="D311" t="s">
+        <v>791</v>
+      </c>
     </row>
     <row r="312" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A312" t="s">
@@ -6759,6 +6900,12 @@
       <c r="B312" t="s">
         <v>425</v>
       </c>
+      <c r="C312" t="s">
+        <v>637</v>
+      </c>
+      <c r="D312" t="s">
+        <v>501</v>
+      </c>
     </row>
     <row r="313" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A313" t="s">
@@ -6767,6 +6914,12 @@
       <c r="B313" t="s">
         <v>426</v>
       </c>
+      <c r="C313" t="s">
+        <v>637</v>
+      </c>
+      <c r="D313" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="314" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A314" t="s">
@@ -6775,6 +6928,12 @@
       <c r="B314" t="s">
         <v>427</v>
       </c>
+      <c r="C314" t="s">
+        <v>637</v>
+      </c>
+      <c r="D314" t="s">
+        <v>531</v>
+      </c>
     </row>
     <row r="315" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A315" t="s">
@@ -6783,6 +6942,12 @@
       <c r="B315" t="s">
         <v>428</v>
       </c>
+      <c r="C315" t="s">
+        <v>536</v>
+      </c>
+      <c r="D315" t="s">
+        <v>806</v>
+      </c>
     </row>
     <row r="316" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A316" t="s">
@@ -6791,6 +6956,12 @@
       <c r="B316" t="s">
         <v>429</v>
       </c>
+      <c r="C316" t="s">
+        <v>435</v>
+      </c>
+      <c r="D316" t="s">
+        <v>503</v>
+      </c>
     </row>
     <row r="317" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A317" t="s">
@@ -6799,6 +6970,9 @@
       <c r="B317" t="s">
         <v>430</v>
       </c>
+      <c r="C317" t="s">
+        <v>431</v>
+      </c>
     </row>
     <row r="318" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A318" t="s">
@@ -6807,6 +6981,12 @@
       <c r="B318" t="s">
         <v>431</v>
       </c>
+      <c r="C318" t="s">
+        <v>432</v>
+      </c>
+      <c r="D318" t="s">
+        <v>815</v>
+      </c>
     </row>
     <row r="319" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A319" t="s">
@@ -6815,6 +6995,12 @@
       <c r="B319" t="s">
         <v>432</v>
       </c>
+      <c r="C319" t="s">
+        <v>435</v>
+      </c>
+      <c r="D319" t="s">
+        <v>814</v>
+      </c>
     </row>
     <row r="320" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A320" t="s">
@@ -6823,56 +7009,95 @@
       <c r="B320" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="321" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C320" t="s">
+        <v>435</v>
+      </c>
+      <c r="D320" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="321" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A321" t="s">
         <v>434</v>
       </c>
       <c r="B321" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="322" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C321" t="s">
+        <v>433</v>
+      </c>
+      <c r="D321" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="322" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A322" t="s">
         <v>435</v>
       </c>
       <c r="B322" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="323" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C322" t="s">
+        <v>536</v>
+      </c>
+      <c r="D322" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="323" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A323" t="s">
         <v>436</v>
       </c>
       <c r="B323" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="324" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C323" t="s">
+        <v>532</v>
+      </c>
+      <c r="D323" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="324" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A324" t="s">
         <v>437</v>
       </c>
       <c r="B324" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="325" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C324" t="s">
+        <v>532</v>
+      </c>
+      <c r="D324" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="325" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A325" t="s">
         <v>438</v>
       </c>
       <c r="B325" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="326" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C325" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="326" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A326" t="s">
         <v>439</v>
       </c>
       <c r="B326" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="327" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C326" t="s">
+        <v>536</v>
+      </c>
+      <c r="D326" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="327" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A327" t="s">
         <v>440</v>
       </c>
@@ -6883,10 +7108,10 @@
         <v>491</v>
       </c>
       <c r="D327" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="328" spans="1:4" x14ac:dyDescent="0.45">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="328" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A328" t="s">
         <v>441</v>
       </c>
@@ -6900,15 +7125,21 @@
         <v>645</v>
       </c>
     </row>
-    <row r="329" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A329" t="s">
         <v>442</v>
       </c>
       <c r="B329" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="330" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C329" t="s">
+        <v>500</v>
+      </c>
+      <c r="D329" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="330" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A330" t="s">
         <v>443</v>
       </c>
@@ -6922,7 +7153,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="331" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A331" t="s">
         <v>444</v>
       </c>
@@ -6933,7 +7164,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="332" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A332" t="s">
         <v>445</v>
       </c>
@@ -6944,7 +7175,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="333" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A333" t="s">
         <v>446</v>
       </c>
@@ -6958,7 +7189,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="334" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A334" t="s">
         <v>447</v>
       </c>
@@ -6969,15 +7200,24 @@
         <v>446</v>
       </c>
     </row>
-    <row r="335" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A335" t="s">
         <v>448</v>
       </c>
       <c r="B335" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="336" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C335" t="s">
+        <v>500</v>
+      </c>
+      <c r="D335" t="s">
+        <v>459</v>
+      </c>
+      <c r="E335" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="336" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A336" t="s">
         <v>449</v>
       </c>
@@ -6985,53 +7225,80 @@
         <v>449</v>
       </c>
       <c r="C336" t="s">
-        <v>15</v>
+        <v>643</v>
       </c>
       <c r="D336" t="s">
         <v>764</v>
       </c>
     </row>
-    <row r="337" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A337" t="s">
         <v>450</v>
       </c>
       <c r="B337" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="338" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C337" t="s">
+        <v>451</v>
+      </c>
+      <c r="D337" t="s">
+        <v>488</v>
+      </c>
+      <c r="E337" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="338" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A338" t="s">
         <v>451</v>
       </c>
       <c r="B338" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="339" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C338" t="s">
+        <v>550</v>
+      </c>
+      <c r="D338" t="s">
+        <v>820</v>
+      </c>
+      <c r="E338" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="339" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A339" t="s">
         <v>452</v>
       </c>
       <c r="B339" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="340" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C339" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="340" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A340" t="s">
         <v>453</v>
       </c>
       <c r="B340" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="341" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C340" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="341" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A341" t="s">
         <v>454</v>
       </c>
       <c r="B341" t="s">
         <v>454</v>
       </c>
-    </row>
-    <row r="342" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C341" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="342" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A342" t="s">
         <v>455</v>
       </c>
@@ -7042,7 +7309,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="343" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A343" t="s">
         <v>456</v>
       </c>
@@ -7053,7 +7320,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="344" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A344" t="s">
         <v>457</v>
       </c>
@@ -7064,7 +7331,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="345" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A345" t="s">
         <v>458</v>
       </c>
@@ -7075,47 +7342,68 @@
         <v>449</v>
       </c>
     </row>
-    <row r="346" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A346" t="s">
         <v>459</v>
       </c>
       <c r="B346" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="347" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C346" t="s">
+        <v>448</v>
+      </c>
+      <c r="D346" t="s">
+        <v>784</v>
+      </c>
+      <c r="E346" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="347" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A347" t="s">
         <v>460</v>
       </c>
       <c r="B347" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="348" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C347" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="348" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A348" t="s">
         <v>461</v>
       </c>
       <c r="B348" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="349" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C348" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="349" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A349" t="s">
         <v>462</v>
       </c>
       <c r="B349" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="350" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C349" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="350" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A350" t="s">
         <v>463</v>
       </c>
       <c r="B350" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="351" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C350" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="351" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A351" t="s">
         <v>464</v>
       </c>
@@ -7126,7 +7414,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="352" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A352" t="s">
         <v>465</v>
       </c>
@@ -7166,6 +7454,9 @@
       <c r="B355" t="s">
         <v>468</v>
       </c>
+      <c r="C355" t="s">
+        <v>451</v>
+      </c>
     </row>
     <row r="356" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A356" t="s">
@@ -7174,6 +7465,9 @@
       <c r="B356" t="s">
         <v>469</v>
       </c>
+      <c r="C356" t="s">
+        <v>552</v>
+      </c>
     </row>
     <row r="357" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A357" t="s">
@@ -7182,6 +7476,9 @@
       <c r="B357" t="s">
         <v>470</v>
       </c>
+      <c r="C357" t="s">
+        <v>561</v>
+      </c>
     </row>
     <row r="358" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A358" t="s">
@@ -7190,6 +7487,9 @@
       <c r="B358" t="s">
         <v>471</v>
       </c>
+      <c r="C358" t="s">
+        <v>550</v>
+      </c>
     </row>
     <row r="359" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A359" t="s">
@@ -7209,6 +7509,9 @@
       <c r="B360" t="s">
         <v>473</v>
       </c>
+      <c r="C360" t="s">
+        <v>546</v>
+      </c>
     </row>
     <row r="361" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A361" t="s">
@@ -7228,6 +7531,9 @@
       <c r="B362" t="s">
         <v>475</v>
       </c>
+      <c r="C362" t="s">
+        <v>613</v>
+      </c>
     </row>
     <row r="363" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A363" t="s">
@@ -7275,6 +7581,9 @@
       <c r="B366" t="s">
         <v>479</v>
       </c>
+      <c r="C366" t="s">
+        <v>592</v>
+      </c>
     </row>
     <row r="367" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A367" t="s">
@@ -7316,6 +7625,9 @@
       <c r="B370" t="s">
         <v>483</v>
       </c>
+      <c r="C370" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="371" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A371" t="s">
@@ -7324,6 +7636,12 @@
       <c r="B371" t="s">
         <v>484</v>
       </c>
+      <c r="C371" t="s">
+        <v>548</v>
+      </c>
+      <c r="D371" t="s">
+        <v>452</v>
+      </c>
     </row>
     <row r="372" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A372" t="s">
@@ -7360,6 +7678,9 @@
       <c r="B374" t="s">
         <v>487</v>
       </c>
+      <c r="C374" t="s">
+        <v>548</v>
+      </c>
     </row>
     <row r="375" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A375" t="s">
@@ -7376,6 +7697,9 @@
       <c r="B376" t="s">
         <v>489</v>
       </c>
+      <c r="C376" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="377" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A377" t="s">
@@ -7399,7 +7723,7 @@
         <v>643</v>
       </c>
       <c r="D378" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="379" spans="1:5" x14ac:dyDescent="0.45">
@@ -7420,6 +7744,12 @@
       <c r="B380" t="s">
         <v>493</v>
       </c>
+      <c r="C380" t="s">
+        <v>561</v>
+      </c>
+      <c r="D380" t="s">
+        <v>801</v>
+      </c>
     </row>
     <row r="381" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A381" t="s">
@@ -7428,6 +7758,9 @@
       <c r="B381" t="s">
         <v>494</v>
       </c>
+      <c r="C381" t="s">
+        <v>558</v>
+      </c>
     </row>
     <row r="382" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A382" t="s">
@@ -7436,6 +7769,9 @@
       <c r="B382" t="s">
         <v>495</v>
       </c>
+      <c r="C382" t="s">
+        <v>558</v>
+      </c>
     </row>
     <row r="383" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A383" t="s">
@@ -7459,15 +7795,18 @@
         <v>643</v>
       </c>
     </row>
-    <row r="385" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="385" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A385" t="s">
         <v>498</v>
       </c>
       <c r="B385" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="386" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C385" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="386" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A386" t="s">
         <v>499</v>
       </c>
@@ -7478,503 +7817,779 @@
         <v>643</v>
       </c>
       <c r="D386" t="s">
-        <v>782</v>
-      </c>
-    </row>
-    <row r="387" spans="1:4" x14ac:dyDescent="0.45">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="387" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A387" t="s">
         <v>500</v>
       </c>
       <c r="B387" t="s">
         <v>500</v>
       </c>
-    </row>
-    <row r="388" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C387" t="s">
+        <v>643</v>
+      </c>
+      <c r="D387" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="388" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A388" t="s">
         <v>501</v>
       </c>
       <c r="B388" t="s">
         <v>501</v>
       </c>
-    </row>
-    <row r="389" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C388" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="389" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A389" t="s">
         <v>502</v>
       </c>
       <c r="B389" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="390" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C389" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="390" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A390" t="s">
         <v>503</v>
       </c>
       <c r="B390" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="391" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C390" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="391" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A391" t="s">
         <v>504</v>
       </c>
       <c r="B391" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="392" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C391" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="392" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A392" t="s">
         <v>505</v>
       </c>
       <c r="B392" t="s">
         <v>505</v>
       </c>
-    </row>
-    <row r="393" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C392" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="393" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A393" t="s">
         <v>506</v>
       </c>
       <c r="B393" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="394" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C393" t="s">
+        <v>507</v>
+      </c>
+      <c r="D393" t="s">
+        <v>795</v>
+      </c>
+      <c r="E393" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="394" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A394" t="s">
         <v>507</v>
       </c>
       <c r="B394" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="395" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C394" t="s">
+        <v>508</v>
+      </c>
+      <c r="D394" t="s">
+        <v>506</v>
+      </c>
+      <c r="E394" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="395" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A395" t="s">
         <v>508</v>
       </c>
       <c r="B395" t="s">
         <v>508</v>
       </c>
-    </row>
-    <row r="396" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C395" t="s">
+        <v>592</v>
+      </c>
+      <c r="D395" t="s">
+        <v>794</v>
+      </c>
+      <c r="E395" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="396" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A396" t="s">
         <v>509</v>
       </c>
       <c r="B396" t="s">
         <v>509</v>
       </c>
-    </row>
-    <row r="397" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C396" t="s">
+        <v>577</v>
+      </c>
+      <c r="D396" t="s">
+        <v>798</v>
+      </c>
+      <c r="E396" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="397" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A397" t="s">
         <v>510</v>
       </c>
       <c r="B397" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="398" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C397" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="398" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A398" t="s">
         <v>511</v>
       </c>
       <c r="B398" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="399" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C398" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="399" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A399" t="s">
         <v>512</v>
       </c>
       <c r="B399" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="400" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C399" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="400" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A400" t="s">
         <v>513</v>
       </c>
       <c r="B400" t="s">
         <v>513</v>
       </c>
-    </row>
-    <row r="401" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C400" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="401" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A401" t="s">
         <v>514</v>
       </c>
       <c r="B401" t="s">
         <v>514</v>
       </c>
-    </row>
-    <row r="402" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C401" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="402" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A402" t="s">
         <v>515</v>
       </c>
       <c r="B402" t="s">
         <v>515</v>
       </c>
-    </row>
-    <row r="403" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C402" t="s">
+        <v>625</v>
+      </c>
+      <c r="D402" t="s">
+        <v>527</v>
+      </c>
+      <c r="E402" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="403" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A403" t="s">
         <v>516</v>
       </c>
       <c r="B403" t="s">
         <v>516</v>
       </c>
-    </row>
-    <row r="404" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C403" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="404" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A404" t="s">
         <v>517</v>
       </c>
       <c r="B404" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="405" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C404" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="405" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A405" t="s">
         <v>518</v>
       </c>
       <c r="B405" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="406" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C405" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="406" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A406" t="s">
         <v>519</v>
       </c>
       <c r="B406" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="407" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C406" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="407" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A407" t="s">
         <v>520</v>
       </c>
       <c r="B407" t="s">
         <v>520</v>
       </c>
-    </row>
-    <row r="408" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C407" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="408" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A408" t="s">
         <v>521</v>
       </c>
       <c r="B408" t="s">
         <v>521</v>
       </c>
-    </row>
-    <row r="409" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C408" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="409" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A409" t="s">
         <v>522</v>
       </c>
       <c r="B409" t="s">
         <v>522</v>
       </c>
-    </row>
-    <row r="410" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C409" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="410" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A410" t="s">
         <v>523</v>
       </c>
       <c r="B410" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="411" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C410" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="411" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A411" t="s">
         <v>524</v>
       </c>
       <c r="B411" t="s">
         <v>524</v>
       </c>
-    </row>
-    <row r="412" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C411" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="412" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A412" t="s">
         <v>525</v>
       </c>
       <c r="B412" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="413" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C412" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="413" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A413" t="s">
         <v>526</v>
       </c>
       <c r="B413" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="414" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C413" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="414" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A414" t="s">
         <v>527</v>
       </c>
       <c r="B414" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="415" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C414" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="415" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A415" t="s">
         <v>528</v>
       </c>
       <c r="B415" t="s">
         <v>528</v>
       </c>
-    </row>
-    <row r="416" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C415" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="416" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A416" t="s">
         <v>529</v>
       </c>
       <c r="B416" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="417" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C416" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="417" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A417" t="s">
         <v>530</v>
       </c>
       <c r="B417" t="s">
         <v>530</v>
       </c>
-    </row>
-    <row r="418" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C417" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="418" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A418" t="s">
         <v>531</v>
       </c>
       <c r="B418" t="s">
         <v>531</v>
       </c>
-    </row>
-    <row r="419" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C418" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="419" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A419" t="s">
         <v>532</v>
       </c>
       <c r="B419" t="s">
         <v>532</v>
       </c>
-    </row>
-    <row r="420" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C419" t="s">
+        <v>643</v>
+      </c>
+      <c r="D419" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="420" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A420" t="s">
         <v>533</v>
       </c>
       <c r="B420" t="s">
         <v>533</v>
       </c>
-    </row>
-    <row r="421" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C420" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="421" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A421" t="s">
         <v>534</v>
       </c>
       <c r="B421" t="s">
         <v>534</v>
       </c>
-    </row>
-    <row r="422" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C421" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="422" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A422" t="s">
         <v>535</v>
       </c>
       <c r="B422" t="s">
         <v>535</v>
       </c>
-    </row>
-    <row r="423" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C422" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="423" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A423" t="s">
         <v>536</v>
       </c>
       <c r="B423" t="s">
         <v>536</v>
       </c>
-    </row>
-    <row r="424" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C423" t="s">
+        <v>643</v>
+      </c>
+      <c r="D423" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="424" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A424" t="s">
         <v>537</v>
       </c>
       <c r="B424" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="425" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C424" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="425" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A425" t="s">
         <v>538</v>
       </c>
       <c r="B425" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="426" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C425" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="426" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A426" t="s">
         <v>539</v>
       </c>
       <c r="B426" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="427" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C426" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="427" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A427" t="s">
         <v>540</v>
       </c>
       <c r="B427" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="428" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C427" t="s">
+        <v>500</v>
+      </c>
+      <c r="D427" t="s">
+        <v>498</v>
+      </c>
+      <c r="E427" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="428" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A428" t="s">
         <v>541</v>
       </c>
       <c r="B428" t="s">
         <v>541</v>
       </c>
-    </row>
-    <row r="429" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C428" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="429" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A429" t="s">
         <v>542</v>
       </c>
       <c r="B429" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="430" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C429" t="s">
+        <v>500</v>
+      </c>
+      <c r="D429" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="430" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A430" t="s">
         <v>543</v>
       </c>
       <c r="B430" t="s">
         <v>543</v>
       </c>
-    </row>
-    <row r="431" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C430" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="431" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A431" t="s">
         <v>544</v>
       </c>
       <c r="B431" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="432" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C431" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="432" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A432" t="s">
         <v>545</v>
       </c>
       <c r="B432" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="433" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C432" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="433" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A433" t="s">
         <v>546</v>
       </c>
       <c r="B433" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="434" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C433" t="s">
+        <v>542</v>
+      </c>
+      <c r="D433" t="s">
+        <v>786</v>
+      </c>
+      <c r="E433" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="434" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A434" t="s">
         <v>547</v>
       </c>
       <c r="B434" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="435" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C434" t="s">
+        <v>550</v>
+      </c>
+      <c r="D434" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="435" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A435" t="s">
         <v>548</v>
       </c>
       <c r="B435" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="436" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C435" t="s">
+        <v>550</v>
+      </c>
+      <c r="D435" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="436" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A436" t="s">
         <v>549</v>
       </c>
       <c r="B436" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="437" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C436" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="437" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A437" t="s">
         <v>550</v>
       </c>
       <c r="B437" t="s">
         <v>550</v>
       </c>
-    </row>
-    <row r="438" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C437" t="s">
+        <v>643</v>
+      </c>
+      <c r="D437" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="438" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A438" t="s">
         <v>551</v>
       </c>
       <c r="B438" t="s">
         <v>551</v>
       </c>
-    </row>
-    <row r="439" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C438" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="439" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A439" t="s">
         <v>552</v>
       </c>
       <c r="B439" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="440" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C439" t="s">
+        <v>553</v>
+      </c>
+      <c r="D439" t="s">
+        <v>803</v>
+      </c>
+      <c r="E439" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="440" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A440" t="s">
         <v>553</v>
       </c>
       <c r="B440" t="s">
         <v>553</v>
       </c>
-    </row>
-    <row r="441" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C440" t="s">
+        <v>643</v>
+      </c>
+      <c r="D440" t="s">
+        <v>802</v>
+      </c>
+      <c r="E440" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="441" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A441" t="s">
         <v>554</v>
       </c>
       <c r="B441" t="s">
         <v>554</v>
       </c>
-    </row>
-    <row r="442" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C441" t="s">
+        <v>643</v>
+      </c>
+      <c r="D441" t="s">
+        <v>787</v>
+      </c>
+      <c r="E441" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="442" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A442" t="s">
         <v>555</v>
       </c>
       <c r="B442" t="s">
         <v>555</v>
       </c>
-    </row>
-    <row r="443" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C442" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="443" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A443" t="s">
         <v>556</v>
       </c>
       <c r="B443" t="s">
         <v>556</v>
       </c>
-    </row>
-    <row r="444" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C443" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="444" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A444" t="s">
         <v>557</v>
       </c>
       <c r="B444" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="445" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C444" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="445" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A445" t="s">
         <v>558</v>
       </c>
       <c r="B445" t="s">
         <v>558</v>
       </c>
-    </row>
-    <row r="446" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C445" t="s">
+        <v>561</v>
+      </c>
+      <c r="D445" t="s">
+        <v>800</v>
+      </c>
+      <c r="E445" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="446" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A446" t="s">
         <v>559</v>
       </c>
       <c r="B446" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="447" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C446" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="447" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A447" t="s">
         <v>560</v>
       </c>
       <c r="B447" t="s">
         <v>560</v>
       </c>
-    </row>
-    <row r="448" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C447" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="448" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A448" t="s">
         <v>561</v>
       </c>
       <c r="B448" t="s">
         <v>561</v>
+      </c>
+      <c r="C448" t="s">
+        <v>592</v>
+      </c>
+      <c r="D448" t="s">
+        <v>799</v>
       </c>
     </row>
     <row r="449" spans="1:5" x14ac:dyDescent="0.45">
@@ -8137,6 +8752,9 @@
       <c r="B461" t="s">
         <v>574</v>
       </c>
+      <c r="C461" t="s">
+        <v>509</v>
+      </c>
     </row>
     <row r="462" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A462" t="s">
@@ -8145,6 +8763,9 @@
       <c r="B462" t="s">
         <v>575</v>
       </c>
+      <c r="C462" t="s">
+        <v>509</v>
+      </c>
     </row>
     <row r="463" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A463" t="s">
@@ -8153,6 +8774,15 @@
       <c r="B463" t="s">
         <v>576</v>
       </c>
+      <c r="C463" t="s">
+        <v>577</v>
+      </c>
+      <c r="D463" t="s">
+        <v>512</v>
+      </c>
+      <c r="E463" t="s">
+        <v>512</v>
+      </c>
     </row>
     <row r="464" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A464" t="s">
@@ -8161,6 +8791,15 @@
       <c r="B464" t="s">
         <v>577</v>
       </c>
+      <c r="C464" t="s">
+        <v>508</v>
+      </c>
+      <c r="D464" t="s">
+        <v>797</v>
+      </c>
+      <c r="E464" t="s">
+        <v>797</v>
+      </c>
     </row>
     <row r="465" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A465" t="s">
@@ -8169,6 +8808,9 @@
       <c r="B465" t="s">
         <v>578</v>
       </c>
+      <c r="C465" t="s">
+        <v>424</v>
+      </c>
     </row>
     <row r="466" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A466" t="s">
@@ -8177,6 +8819,9 @@
       <c r="B466" t="s">
         <v>579</v>
       </c>
+      <c r="C466" t="s">
+        <v>424</v>
+      </c>
     </row>
     <row r="467" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A467" t="s">
@@ -8185,6 +8830,9 @@
       <c r="B467" t="s">
         <v>580</v>
       </c>
+      <c r="C467" t="s">
+        <v>424</v>
+      </c>
     </row>
     <row r="468" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A468" t="s">
@@ -8193,6 +8841,9 @@
       <c r="B468" t="s">
         <v>581</v>
       </c>
+      <c r="C468" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="469" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A469" t="s">
@@ -8201,6 +8852,9 @@
       <c r="B469" t="s">
         <v>582</v>
       </c>
+      <c r="C469" t="s">
+        <v>435</v>
+      </c>
     </row>
     <row r="470" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A470" t="s">
@@ -8209,6 +8863,9 @@
       <c r="B470" t="s">
         <v>583</v>
       </c>
+      <c r="C470" t="s">
+        <v>584</v>
+      </c>
     </row>
     <row r="471" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A471" t="s">
@@ -8217,6 +8874,12 @@
       <c r="B471" t="s">
         <v>584</v>
       </c>
+      <c r="C471" t="s">
+        <v>506</v>
+      </c>
+      <c r="D471" t="s">
+        <v>583</v>
+      </c>
     </row>
     <row r="472" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A472" t="s">
@@ -8290,10 +8953,10 @@
         <v>421</v>
       </c>
       <c r="D477" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="E477" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="478" spans="1:5" x14ac:dyDescent="0.45">
@@ -8303,6 +8966,9 @@
       <c r="B478" t="s">
         <v>591</v>
       </c>
+      <c r="C478" t="s">
+        <v>592</v>
+      </c>
     </row>
     <row r="479" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A479" t="s">
@@ -8311,6 +8977,12 @@
       <c r="B479" t="s">
         <v>592</v>
       </c>
+      <c r="C479" t="s">
+        <v>643</v>
+      </c>
+      <c r="D479" t="s">
+        <v>793</v>
+      </c>
     </row>
     <row r="480" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A480" t="s">
@@ -8367,7 +9039,7 @@
         <v>499</v>
       </c>
       <c r="D484" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="485" spans="1:5" x14ac:dyDescent="0.45">
@@ -8463,6 +9135,9 @@
       <c r="B492" t="s">
         <v>605</v>
       </c>
+      <c r="C492" t="s">
+        <v>617</v>
+      </c>
     </row>
     <row r="493" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A493" t="s">
@@ -8471,6 +9146,9 @@
       <c r="B493" t="s">
         <v>606</v>
       </c>
+      <c r="C493" t="s">
+        <v>436</v>
+      </c>
     </row>
     <row r="494" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A494" t="s">
@@ -8479,6 +9157,9 @@
       <c r="B494" t="s">
         <v>607</v>
       </c>
+      <c r="C494" t="s">
+        <v>437</v>
+      </c>
     </row>
     <row r="495" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A495" t="s">
@@ -8549,7 +9230,7 @@
         <v>616</v>
       </c>
       <c r="D500" t="s">
-        <v>778</v>
+        <v>821</v>
       </c>
     </row>
     <row r="501" spans="1:5" x14ac:dyDescent="0.45">
@@ -8601,6 +9282,12 @@
       <c r="B504" t="s">
         <v>617</v>
       </c>
+      <c r="C504" t="s">
+        <v>536</v>
+      </c>
+      <c r="D504" t="s">
+        <v>818</v>
+      </c>
     </row>
     <row r="505" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A505" t="s">
@@ -8609,6 +9296,9 @@
       <c r="B505" t="s">
         <v>618</v>
       </c>
+      <c r="C505" t="s">
+        <v>619</v>
+      </c>
     </row>
     <row r="506" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A506" t="s">
@@ -8617,6 +9307,15 @@
       <c r="B506" t="s">
         <v>619</v>
       </c>
+      <c r="C506" t="s">
+        <v>428</v>
+      </c>
+      <c r="D506" t="s">
+        <v>807</v>
+      </c>
+      <c r="E506" t="s">
+        <v>808</v>
+      </c>
     </row>
     <row r="507" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A507" t="s">
@@ -8625,6 +9324,9 @@
       <c r="B507" t="s">
         <v>620</v>
       </c>
+      <c r="C507" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="508" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A508" t="s">
@@ -8633,6 +9335,9 @@
       <c r="B508" t="s">
         <v>621</v>
       </c>
+      <c r="C508" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="509" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A509" t="s">
@@ -8641,6 +9346,9 @@
       <c r="B509" t="s">
         <v>622</v>
       </c>
+      <c r="C509" t="s">
+        <v>624</v>
+      </c>
     </row>
     <row r="510" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A510" t="s">
@@ -8649,6 +9357,9 @@
       <c r="B510" t="s">
         <v>623</v>
       </c>
+      <c r="C510" t="s">
+        <v>624</v>
+      </c>
     </row>
     <row r="511" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A511" t="s">
@@ -8657,6 +9368,15 @@
       <c r="B511" t="s">
         <v>624</v>
       </c>
+      <c r="C511" t="s">
+        <v>625</v>
+      </c>
+      <c r="D511" t="s">
+        <v>811</v>
+      </c>
+      <c r="E511" t="s">
+        <v>811</v>
+      </c>
     </row>
     <row r="512" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A512" t="s">
@@ -8665,6 +9385,15 @@
       <c r="B512" t="s">
         <v>625</v>
       </c>
+      <c r="C512" t="s">
+        <v>626</v>
+      </c>
+      <c r="D512" t="s">
+        <v>810</v>
+      </c>
+      <c r="E512" t="s">
+        <v>810</v>
+      </c>
     </row>
     <row r="513" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A513" t="s">
@@ -8673,6 +9402,15 @@
       <c r="B513" t="s">
         <v>626</v>
       </c>
+      <c r="C513" t="s">
+        <v>428</v>
+      </c>
+      <c r="D513" t="s">
+        <v>809</v>
+      </c>
+      <c r="E513" t="s">
+        <v>809</v>
+      </c>
     </row>
     <row r="514" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A514" t="s">
@@ -8681,6 +9419,9 @@
       <c r="B514" t="s">
         <v>627</v>
       </c>
+      <c r="C514" t="s">
+        <v>440</v>
+      </c>
     </row>
     <row r="515" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A515" t="s">
@@ -8714,6 +9455,12 @@
       <c r="B517" t="s">
         <v>630</v>
       </c>
+      <c r="C517" t="s">
+        <v>632</v>
+      </c>
+      <c r="D517" t="s">
+        <v>631</v>
+      </c>
     </row>
     <row r="518" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A518" t="s">
@@ -8722,6 +9469,9 @@
       <c r="B518" t="s">
         <v>631</v>
       </c>
+      <c r="C518" t="s">
+        <v>630</v>
+      </c>
     </row>
     <row r="519" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A519" t="s">
@@ -8730,6 +9480,12 @@
       <c r="B519" t="s">
         <v>632</v>
       </c>
+      <c r="C519" t="s">
+        <v>424</v>
+      </c>
+      <c r="D519" t="s">
+        <v>792</v>
+      </c>
     </row>
     <row r="520" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A520" t="s">
@@ -8738,6 +9494,9 @@
       <c r="B520" t="s">
         <v>633</v>
       </c>
+      <c r="C520" t="s">
+        <v>635</v>
+      </c>
     </row>
     <row r="521" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A521" t="s">
@@ -8746,6 +9505,9 @@
       <c r="B521" t="s">
         <v>634</v>
       </c>
+      <c r="C521" t="s">
+        <v>439</v>
+      </c>
     </row>
     <row r="522" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A522" t="s">
@@ -8754,6 +9516,12 @@
       <c r="B522" t="s">
         <v>635</v>
       </c>
+      <c r="C522" t="s">
+        <v>435</v>
+      </c>
+      <c r="D522" t="s">
+        <v>813</v>
+      </c>
     </row>
     <row r="523" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A523" t="s">
@@ -8772,6 +9540,12 @@
       </c>
       <c r="B524" t="s">
         <v>637</v>
+      </c>
+      <c r="C524" t="s">
+        <v>643</v>
+      </c>
+      <c r="D524" t="s">
+        <v>789</v>
       </c>
     </row>
     <row r="525" spans="1:5" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Database creation code completed!
</commit_message>
<xml_diff>
--- a/FlowTracker.xlsx
+++ b/FlowTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cbnor\Documents\Full Body Flow Model Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC7C260-7244-4A4E-826A-0FEC04CA6F9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69BC0DE3-368E-4D73-A742-91A1E6D74003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2206" uniqueCount="821">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2207" uniqueCount="821">
   <si>
     <t>Filename</t>
   </si>
@@ -2885,9 +2885,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G579"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A536" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E549" sqref="E549"/>
+      <selection pane="bottomLeft" activeCell="G554" sqref="G554"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10042,6 +10042,9 @@
       </c>
       <c r="C553" t="s">
         <v>681</v>
+      </c>
+      <c r="G553" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="554" spans="1:7" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Revert "Vessel Fitting Work"
This reverts commit 7b62a3a32eb9a6bb66bf1a60e3a1da449ee7064a.
</commit_message>
<xml_diff>
--- a/FlowTracker.xlsx
+++ b/FlowTracker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cbnor\Documents\Full Body Flow Model Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB776846-B44F-493C-91AD-1BEE08D37A36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB023EA-CB07-4288-872E-4546F9A33262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2213" uniqueCount="822">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2206" uniqueCount="822">
   <si>
     <t>Filename</t>
   </si>
@@ -2889,8 +2889,8 @@
   <dimension ref="A1:G579"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3164,11 +3164,8 @@
       <c r="C16" t="s">
         <v>56</v>
       </c>
-      <c r="G16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -3178,11 +3175,8 @@
       <c r="C17" t="s">
         <v>95</v>
       </c>
-      <c r="G17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -3192,11 +3186,8 @@
       <c r="C18" t="s">
         <v>75</v>
       </c>
-      <c r="G18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -3206,11 +3197,8 @@
       <c r="C19" t="s">
         <v>75</v>
       </c>
-      <c r="G19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -3220,11 +3208,8 @@
       <c r="C20" t="s">
         <v>52</v>
       </c>
-      <c r="G20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -3237,11 +3222,8 @@
       <c r="D21" t="s">
         <v>43</v>
       </c>
-      <c r="G21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -3254,11 +3236,8 @@
       <c r="D22" t="s">
         <v>38</v>
       </c>
-      <c r="G22" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -3269,7 +3248,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -3280,7 +3259,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -3291,7 +3270,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -3302,7 +3281,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -3313,7 +3292,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -3327,7 +3306,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -3338,7 +3317,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -3352,7 +3331,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -3366,7 +3345,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>49</v>
       </c>

</xml_diff>

<commit_message>
Revert "Revert "Vessel Fitting Work""
This reverts commit 1e046670d258fab0c04eeb1942e735bb55291ca4.
</commit_message>
<xml_diff>
--- a/FlowTracker.xlsx
+++ b/FlowTracker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cbnor\Documents\Full Body Flow Model Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB023EA-CB07-4288-872E-4546F9A33262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB776846-B44F-493C-91AD-1BEE08D37A36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2206" uniqueCount="822">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2213" uniqueCount="822">
   <si>
     <t>Filename</t>
   </si>
@@ -2889,8 +2889,8 @@
   <dimension ref="A1:G579"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3164,8 +3164,11 @@
       <c r="C16" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="G16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -3175,8 +3178,11 @@
       <c r="C17" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="G17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -3186,8 +3192,11 @@
       <c r="C18" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="G18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -3197,8 +3206,11 @@
       <c r="C19" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="G19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -3208,8 +3220,11 @@
       <c r="C20" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="G20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -3222,8 +3237,11 @@
       <c r="D21" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="G21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -3236,8 +3254,11 @@
       <c r="D22" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="G22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -3248,7 +3269,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -3259,7 +3280,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -3270,7 +3291,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -3281,7 +3302,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -3292,7 +3313,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -3306,7 +3327,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -3317,7 +3338,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -3331,7 +3352,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -3345,7 +3366,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>49</v>
       </c>

</xml_diff>

<commit_message>
In office Monday work
</commit_message>
<xml_diff>
--- a/FlowTracker.xlsx
+++ b/FlowTracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cassidy.Northway\RemoteGit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEBF82B1-AC01-4321-B1B4-3217151E35CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0879CCFA-F894-48DD-B931-D55ECF9DB516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="arteries" sheetId="1" r:id="rId1"/>
@@ -2896,7 +2896,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D2" sqref="D2"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>